<commit_message>
Alterada a etapa 12
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
+++ b/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
@@ -125,7 +125,7 @@
     <t>Usuário do Sistema visualiza formulário de informações complementares</t>
   </si>
   <si>
-    <t>SYSTEM apresenta campos: Tipo de Cliente (padrão 'A') e Quantidade (vazio)</t>
+    <t>SYSTEM apresenta campos: Tipo de Cliente e Quantidade</t>
   </si>
   <si>
     <t>Usuário do Sistema altera para tipo de cliente B</t>
@@ -134,64 +134,64 @@
     <t>SYSTEM registra o tipo de cliente selecionado</t>
   </si>
   <si>
+    <t>Usuário do Sistema informa a quantidade de produtos menor que 100 unidades</t>
+  </si>
+  <si>
+    <t>SYSTEM aplica fator de desconto para quantidade &lt; 100: Cliente A (0,90), B (0,85), C (0,80)</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
+  </si>
+  <si>
+    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema é redirecionado para página de resultado</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema mantém seleção padrão do tipo de cliente A</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
+  </si>
+  <si>
+    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema altera para tipo de cliente C</t>
+  </si>
+  <si>
     <t>Usuário do Sistema informa a quantidade de produtos</t>
   </si>
   <si>
     <t>SYSTEM registra a quantidade informada</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
-  </si>
-  <si>
-    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema é redirecionado para página de resultado</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
-  </si>
-  <si>
-    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema altera para tipo de cliente C</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos menor que 100 unidades</t>
-  </si>
-  <si>
-    <t>SYSTEM aplica fator de desconto para quantidade &lt; 100: Cliente A (0,90), B (0,85), C (0,80)</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema mantém seleção padrão do tipo de cliente A</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
-  </si>
-  <si>
-    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
   </si>
   <si>
     <t>TC4</t>
@@ -2057,7 +2057,7 @@
         <v>7.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>

</xml_diff>

<commit_message>
Melhoria do fluxo alternativo 7
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
+++ b/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="67">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -128,10 +128,76 @@
     <t>SYSTEM apresenta campos: Tipo de Cliente e Quantidade</t>
   </si>
   <si>
+    <t>Usuário do Sistema mantém seleção padrão do tipo de cliente A</t>
+  </si>
+  <si>
+    <t>SYSTEM registra o tipo de cliente selecionado</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema informa a quantidade de produtos</t>
+  </si>
+  <si>
+    <t>SYSTEM registra a quantidade informada</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
+  </si>
+  <si>
+    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema é redirecionado para página de resultado</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema seleciona tipo de cliente se desejar alterar</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
+  </si>
+  <si>
+    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
     <t>Usuário do Sistema altera para tipo de cliente B</t>
   </si>
   <si>
-    <t>SYSTEM registra o tipo de cliente selecionado</t>
+    <t>Usuário do Sistema informa a quantidade de produtos entre 100 e 999 unidades</t>
+  </si>
+  <si>
+    <t>SYSTEM aplica fator de desconto para 100 &lt;= quantidade &lt; 1000: Cliente A (0,95), B (0,90), C (0,85)</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema altera para tipo de cliente C</t>
   </si>
   <si>
     <t>Usuário do Sistema informa a quantidade de produtos menor que 100 unidades</t>
@@ -140,79 +206,13 @@
     <t>SYSTEM aplica fator de desconto para quantidade &lt; 100: Cliente A (0,90), B (0,85), C (0,80)</t>
   </si>
   <si>
-    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
-  </si>
-  <si>
-    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema é redirecionado para página de resultado</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
-  </si>
-  <si>
-    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema mantém seleção padrão do tipo de cliente A</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
-  </si>
-  <si>
-    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema altera para tipo de cliente C</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos</t>
-  </si>
-  <si>
-    <t>SYSTEM registra a quantidade informada</t>
-  </si>
-  <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona tipo de cliente se desejar alterar</t>
+    <t>TC5</t>
   </si>
   <si>
     <t>Usuário do Sistema informa a quantidade de produtos menor ou igual a zero</t>
   </si>
   <si>
     <t>SYSTEM exibe mensagem 'A quantidade informada deve ser maior ou igual a 01 (um)!' (MSG002)</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos entre 100 e 999 unidades</t>
-  </si>
-  <si>
-    <t>SYSTEM aplica fator de desconto para 100 &lt;= quantidade &lt; 1000: Cliente A (0,95), B (0,90), C (0,85)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F93"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -2089,106 +2089,6 @@
         <v>2</v>
       </c>
       <c r="F93" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B94" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C94" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D94" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E94" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F94" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B95" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C95" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D95" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E95" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F95" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B96" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C96" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D96" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E96" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F96" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B97" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C97" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D97" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E97" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F97" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B98" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="C98" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D98" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E98" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F98" t="s" s="8">
         <v>2</v>
       </c>
     </row>
@@ -2209,7 +2109,6 @@
     <mergeCell ref="B79:F79"/>
     <mergeCell ref="B83:D83"/>
     <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B98:F98"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Refatorando o fluxo alternativo 7
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
+++ b/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="67">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -128,91 +128,91 @@
     <t>SYSTEM apresenta campos: Tipo de Cliente e Quantidade</t>
   </si>
   <si>
+    <t>Usuário do Sistema altera para tipo de cliente C</t>
+  </si>
+  <si>
+    <t>SYSTEM registra o tipo de cliente selecionado</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema informa a quantidade de produtos</t>
+  </si>
+  <si>
+    <t>SYSTEM registra a quantidade informada</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
+  </si>
+  <si>
+    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema é redirecionado para página de resultado</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
     <t>Usuário do Sistema mantém seleção padrão do tipo de cliente A</t>
   </si>
   <si>
-    <t>SYSTEM registra o tipo de cliente selecionado</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos</t>
-  </si>
-  <si>
-    <t>SYSTEM registra a quantidade informada</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
-  </si>
-  <si>
-    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema é redirecionado para página de resultado</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
-  </si>
-  <si>
-    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
-  </si>
-  <si>
-    <t>TC2</t>
+    <t>Usuário do Sistema informa a quantidade de produtos menor ou igual a zero</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem 'A quantidade informada deve ser maior ou igual a 01 (um)!' (MSG002)</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema altera para tipo de cliente B</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
+  </si>
+  <si>
+    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
+  </si>
+  <si>
+    <t>TC4</t>
   </si>
   <si>
     <t>Usuário do Sistema seleciona tipo de cliente se desejar alterar</t>
   </si>
   <si>
-    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
-  </si>
-  <si>
-    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema altera para tipo de cliente B</t>
-  </si>
-  <si>
     <t>Usuário do Sistema informa a quantidade de produtos entre 100 e 999 unidades</t>
   </si>
   <si>
     <t>SYSTEM aplica fator de desconto para 100 &lt;= quantidade &lt; 1000: Cliente A (0,95), B (0,90), C (0,85)</t>
   </si>
   <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema altera para tipo de cliente C</t>
+    <t>TC5</t>
   </si>
   <si>
     <t>Usuário do Sistema informa a quantidade de produtos menor que 100 unidades</t>
   </si>
   <si>
     <t>SYSTEM aplica fator de desconto para quantidade &lt; 100: Cliente A (0,90), B (0,85), C (0,80)</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos menor ou igual a zero</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'A quantidade informada deve ser maior ou igual a 01 (um)!' (MSG002)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +408,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -1057,7 +1057,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s" s="7">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E36" t="s" s="6">
         <v>2</v>
@@ -1077,7 +1077,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s" s="7">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E37" t="s" s="6">
         <v>2</v>
@@ -1086,180 +1086,180 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B38" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C38" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E38" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B39" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C39" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D39" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E39" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F39" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="38"/>
+    <row r="39"/>
     <row r="40">
-      <c r="A40" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B40" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C40" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E40" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F40" t="s" s="6">
+      <c r="A40" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s" s="4">
+        <v>56</v>
+      </c>
+      <c r="C40" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E40" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F40" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B41" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="C41" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E41" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F41" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42"/>
-    <row r="43"/>
+      <c r="A41" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E41" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F41" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B42" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E42" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E43" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F43" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
     <row r="44">
-      <c r="A44" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B44" t="s" s="4">
-        <v>56</v>
-      </c>
-      <c r="C44" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D44" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E44" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F44" t="s" s="4">
+      <c r="A44" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B44" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="C44" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="E44" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B45" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C45" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E45" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F45" t="s" s="9">
+      <c r="A45" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B45" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="C45" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D45" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="E45" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B46" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C46" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D46" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E46" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F46" t="s" s="8">
+      <c r="A46" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B46" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C46" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B47" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C47" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D47" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E47" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F47" t="s" s="5">
-        <v>25</v>
+      <c r="A47" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B47" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C47" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D47" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E47" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n" s="10">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="B48" t="s" s="7">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C48" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D48" t="s" s="7">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E48" t="s" s="6">
         <v>2</v>
@@ -1270,16 +1270,16 @@
     </row>
     <row r="49">
       <c r="A49" t="n" s="10">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D49" t="s" s="7">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E49" t="s" s="6">
         <v>2</v>
@@ -1290,16 +1290,16 @@
     </row>
     <row r="50">
       <c r="A50" t="n" s="10">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="B50" t="s" s="7">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D50" t="s" s="7">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E50" t="s" s="6">
         <v>2</v>
@@ -1310,16 +1310,16 @@
     </row>
     <row r="51">
       <c r="A51" t="n" s="10">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="B51" t="s" s="7">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C51" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D51" t="s" s="7">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="E51" t="s" s="6">
         <v>2</v>
@@ -1330,16 +1330,16 @@
     </row>
     <row r="52">
       <c r="A52" t="n" s="10">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
       <c r="B52" t="s" s="7">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D52" t="s" s="7">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E52" t="s" s="6">
         <v>2</v>
@@ -1350,16 +1350,16 @@
     </row>
     <row r="53">
       <c r="A53" t="n" s="10">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="B53" t="s" s="7">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D53" t="s" s="7">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E53" t="s" s="6">
         <v>2</v>
@@ -1370,16 +1370,16 @@
     </row>
     <row r="54">
       <c r="A54" t="n" s="10">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="B54" t="s" s="7">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C54" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D54" t="s" s="7">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E54" t="s" s="6">
         <v>2</v>
@@ -1390,16 +1390,16 @@
     </row>
     <row r="55">
       <c r="A55" t="n" s="10">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D55" t="s" s="7">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E55" t="s" s="6">
         <v>2</v>
@@ -1409,199 +1409,199 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B56" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C56" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D56" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E56" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F56" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B57" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C57" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D57" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E57" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F57" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B58" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C58" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D58" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E58" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F58" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+      <c r="A56" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="B56" t="s" s="8">
+        <v>51</v>
+      </c>
+      <c r="C56" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57"/>
+    <row r="58"/>
     <row r="59">
-      <c r="A59" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B59" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C59" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D59" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E59" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F59" t="s" s="6">
+      <c r="A59" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B59" t="s" s="4">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D59" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F59" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B60" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="C60" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E60" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F60" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61"/>
-    <row r="62"/>
+      <c r="A60" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B60" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C60" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F60" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B61" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E61" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C62" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E62" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F62" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
     <row r="63">
-      <c r="A63" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B63" t="s" s="4">
-        <v>60</v>
-      </c>
-      <c r="C63" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D63" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F63" t="s" s="4">
+      <c r="A63" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B63" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="C63" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="E63" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F63" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F64" t="s" s="9">
+      <c r="A64" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B64" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="C64" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="E64" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B65" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F65" t="s" s="8">
+      <c r="A65" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B65" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C65" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="E65" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B66" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C66" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D66" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E66" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F66" t="s" s="5">
-        <v>25</v>
+      <c r="A66" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B66" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E66" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F66" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n" s="10">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="B67" t="s" s="7">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C67" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D67" t="s" s="7">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E67" t="s" s="6">
         <v>2</v>
@@ -1612,16 +1612,16 @@
     </row>
     <row r="68">
       <c r="A68" t="n" s="10">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E68" t="s" s="6">
         <v>2</v>
@@ -1632,16 +1632,16 @@
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1652,16 +1652,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1672,16 +1672,16 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1692,16 +1692,16 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E72" t="s" s="6">
         <v>2</v>
@@ -1712,16 +1712,16 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E73" t="s" s="6">
         <v>2</v>
@@ -1732,16 +1732,16 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C74" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="E74" t="s" s="6">
         <v>2</v>
@@ -1751,199 +1751,199 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B75" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C75" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D75" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E75" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F75" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B76" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C76" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D76" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E76" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F76" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B77" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C77" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D77" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E77" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F77" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+      <c r="A75" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="B75" t="s" s="8">
+        <v>51</v>
+      </c>
+      <c r="C75" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E75" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F75" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76"/>
+    <row r="77"/>
     <row r="78">
-      <c r="A78" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B78" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D78" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F78" t="s" s="6">
+      <c r="A78" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B78" t="s" s="4">
+        <v>64</v>
+      </c>
+      <c r="C78" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E78" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F78" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B79" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="C79" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E79" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F79" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80"/>
-    <row r="81"/>
+      <c r="A79" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B79" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C79" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E79" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F79" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B80" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C80" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F80" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B81" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C81" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D81" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E81" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F81" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
     <row r="82">
-      <c r="A82" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B82" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="C82" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D82" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F82" t="s" s="4">
+      <c r="A82" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B82" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="C82" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="E82" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F82" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F83" t="s" s="9">
+      <c r="A83" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B83" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="C83" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="E83" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B84" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="8">
+      <c r="A84" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B84" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="E84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B85" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C85" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D85" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E85" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F85" t="s" s="5">
-        <v>25</v>
+      <c r="A85" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B85" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1954,16 +1954,16 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>2.0</v>
+        <v>6.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -1974,16 +1974,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -1994,16 +1994,16 @@
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2014,16 +2014,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>5.0</v>
+        <v>9.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2034,16 +2034,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2054,16 +2054,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2074,21 +2074,41 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>8.0</v>
+        <v>12.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="F93" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s" s="8">
+        <v>50</v>
+      </c>
+      <c r="B94" t="s" s="8">
+        <v>51</v>
+      </c>
+      <c r="C94" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E94" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F94" t="s" s="8">
         <v>2</v>
       </c>
     </row>
@@ -2100,15 +2120,15 @@
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="B60:F60"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B79:F79"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B75:F75"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B80:F80"/>
+    <mergeCell ref="B94:F94"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizacao do UC001; Criacao do CRUD de produto
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
+++ b/output/xlsx/UC001 - Calcular Desconto de Produto--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="65">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -41,7 +41,7 @@
     <t>Reduced (Greedy Heuristic - Transition Coverage)</t>
   </si>
   <si>
-    <t>Size: 5 test case(s))</t>
+    <t>Size: 4 test case(s))</t>
   </si>
   <si>
     <t xml:space="preserve">Creation Date: </t>
@@ -128,91 +128,85 @@
     <t>SYSTEM apresenta campos: Tipo de Cliente e Quantidade</t>
   </si>
   <si>
+    <t>Usuário do Sistema seleciona tipo de cliente se desejar alterar</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta o tipo de cliente selecionado</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
+  </si>
+  <si>
+    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
+  </si>
+  <si>
+    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema é redirecionado para página de resultado</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
+  </si>
+  <si>
+    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
     <t>Usuário do Sistema altera para tipo de cliente C</t>
   </si>
   <si>
-    <t>SYSTEM registra o tipo de cliente selecionado</t>
-  </si>
-  <si>
     <t>Usuário do Sistema informa a quantidade de produtos</t>
   </si>
   <si>
-    <t>SYSTEM registra a quantidade informada</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema clica no botão 'Calcular Desconto!'</t>
-  </si>
-  <si>
-    <t>SYSTEM processa o cálculo do desconto baseado no tipo de cliente e quantidade</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema é redirecionado para página de resultado</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'Valor do desconto calculado com sucesso!'</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza resultado do cálculo com todos os detalhes</t>
-  </si>
-  <si>
-    <t>SYSTEM apresenta: tipo de cliente, quantidade, fator de desconto e valor final</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema visualiza dados originais do produto para conferência</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe botão 'Realizar Novo Cálculo'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>Usuário visualiza o desconto calculado com todos os detalhes e pode realizar novo cálculo</t>
-  </si>
-  <si>
-    <t>TC2</t>
+    <t>SYSTEM apresenta a quantidade informada</t>
+  </si>
+  <si>
+    <t>SYSTEM exibe mensagem 'A quantidade informada deve ser maior ou igual a 01 (um)!' (MSG002)</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema altera para tipo de cliente B</t>
+  </si>
+  <si>
+    <t>Usuário do Sistema informa a quantidade de produtos menor que 100 unidades</t>
+  </si>
+  <si>
+    <t>SYSTEM aplica fator de desconto para quantidade &lt; 100: Cliente A (0,90), B (0,85), C (0,80)</t>
+  </si>
+  <si>
+    <t>TC4</t>
   </si>
   <si>
     <t>Usuário do Sistema mantém seleção padrão do tipo de cliente A</t>
   </si>
   <si>
-    <t>Usuário do Sistema informa a quantidade de produtos menor ou igual a zero</t>
-  </si>
-  <si>
-    <t>SYSTEM exibe mensagem 'A quantidade informada deve ser maior ou igual a 01 (um)!' (MSG002)</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema altera para tipo de cliente B</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos igual ou maior que 1000 unidades</t>
-  </si>
-  <si>
-    <t>SYSTEM aplica fator de desconto para quantidade &gt;= 1000: Cliente A (1,00), B (0,95), C (0,90)</t>
-  </si>
-  <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema seleciona tipo de cliente se desejar alterar</t>
-  </si>
-  <si>
     <t>Usuário do Sistema informa a quantidade de produtos entre 100 e 999 unidades</t>
   </si>
   <si>
     <t>SYSTEM aplica fator de desconto para 100 &lt;= quantidade &lt; 1000: Cliente A (0,95), B (0,90), C (0,85)</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>Usuário do Sistema informa a quantidade de produtos menor que 100 unidades</t>
-  </si>
-  <si>
-    <t>SYSTEM aplica fator de desconto para quantidade &lt; 100: Cliente A (0,90), B (0,85), C (0,80)</t>
   </si>
 </sst>
 </file>
@@ -408,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F94"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -1057,7 +1051,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s" s="7">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="E36" t="s" s="6">
         <v>2</v>
@@ -1077,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s" s="7">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E37" t="s" s="6">
         <v>2</v>
@@ -1093,7 +1087,7 @@
         <v>12</v>
       </c>
       <c r="B40" t="s" s="4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s" s="4">
         <v>14</v>
@@ -1293,7 +1287,7 @@
         <v>7.0</v>
       </c>
       <c r="B50" t="s" s="7">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C50" t="s" s="6">
         <v>2</v>
@@ -1313,13 +1307,13 @@
         <v>8.0</v>
       </c>
       <c r="B51" t="s" s="7">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C51" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D51" t="s" s="7">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E51" t="s" s="6">
         <v>2</v>
@@ -1435,7 +1429,7 @@
         <v>12</v>
       </c>
       <c r="B59" t="s" s="4">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C59" t="s" s="4">
         <v>14</v>
@@ -1635,7 +1629,7 @@
         <v>7.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
@@ -1655,13 +1649,13 @@
         <v>8.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1681,434 +1675,12 @@
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="F71" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B72" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C72" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D72" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E72" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F72" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B73" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C73" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E73" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F73" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B74" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C74" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D74" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E74" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F74" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B75" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="C75" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D75" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E75" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F75" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78">
-      <c r="A78" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B78" t="s" s="4">
-        <v>64</v>
-      </c>
-      <c r="C78" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D78" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E78" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F78" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B79" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C79" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E79" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F79" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B80" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C80" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D80" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E80" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F80" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B81" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C81" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D81" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E81" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F81" t="s" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B82" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C82" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="E82" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F82" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B83" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C83" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="E83" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F83" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B84" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="C84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="E84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B85" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F85" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B86" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C86" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D86" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E86" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F86" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B87" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C87" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E87" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F87" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B88" t="s" s="7">
-        <v>53</v>
-      </c>
-      <c r="C88" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E88" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F88" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B89" t="s" s="7">
-        <v>65</v>
-      </c>
-      <c r="C89" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="E89" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F89" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B90" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C90" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D90" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E90" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F90" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B91" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C91" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D91" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E91" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F91" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B92" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C92" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D92" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E92" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F92" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B93" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C93" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D93" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E93" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F93" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B94" t="s" s="8">
-        <v>51</v>
-      </c>
-      <c r="C94" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D94" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E94" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F94" t="s" s="8">
         <v>2</v>
       </c>
     </row>
@@ -2125,10 +1697,6 @@
     <mergeCell ref="B56:F56"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B75:F75"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B80:F80"/>
-    <mergeCell ref="B94:F94"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>